<commit_message>
-Updated the website to the one provided - Fix the date on boarderd - added a use application/browser
</commit_message>
<xml_diff>
--- a/.local/NWU Tech Trends Data.xlsx
+++ b/.local/NWU Tech Trends Data.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brand\OneDrive\Desktop\JM Repo\JM Work Repo\NWU\Modules\2024 CMPG323\Project 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B432EAD3-C6FE-4098-AA29-885124F46384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A866E17-E39B-4670-9D07-05D4DA3B5C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CD795CCD-582F-4BD0-AF39-75E63E90AABB}"/>
+    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15720" xr2:uid="{CD795CCD-582F-4BD0-AF39-75E63E90AABB}"/>
   </bookViews>
   <sheets>
     <sheet name="Clients" sheetId="1" r:id="rId1"/>
     <sheet name="Projects" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="348">
   <si>
     <t>ClientID</t>
   </si>
@@ -51,457 +51,607 @@
     <t>DateOnboarded</t>
   </si>
   <si>
+    <t>Test Passed</t>
+  </si>
+  <si>
+    <t>68c53a7b-2b9e-4dbe-a536-4d1a2f27a0b7</t>
+  </si>
+  <si>
     <t>Tech Innovators</t>
   </si>
   <si>
     <t>contact1@techinnovators.com</t>
   </si>
   <si>
+    <t>002023/01/15</t>
+  </si>
+  <si>
+    <t>77af89a2-7c76-4263-a8ee-2b25541f89af</t>
+  </si>
+  <si>
     <t>Data Dynamics</t>
   </si>
   <si>
     <t>contact2@datadynamics.com</t>
   </si>
   <si>
+    <t>002023/01/16</t>
+  </si>
+  <si>
+    <t>f5a92c1a-59b0-496f-8d17-64bdf59d3f6a</t>
+  </si>
+  <si>
     <t>Cloud Solutions</t>
   </si>
   <si>
     <t>contact3@cloudsolutions.com</t>
   </si>
   <si>
+    <t>002023/01/17</t>
+  </si>
+  <si>
+    <t>c1c1fbb6-9a94-41b7-94f8-7a621aa1a7b6</t>
+  </si>
+  <si>
     <t>AI Pioneers</t>
   </si>
   <si>
     <t>contact4@aipioneers.com</t>
   </si>
   <si>
+    <t>002023/01/18</t>
+  </si>
+  <si>
+    <t>9e58f2fa-d8a8-46c7-988a-2bb0c9c78f94</t>
+  </si>
+  <si>
     <t>Green Energy Corp</t>
   </si>
   <si>
     <t>contact5@greenenergy.com</t>
   </si>
   <si>
+    <t>002023/01/19</t>
+  </si>
+  <si>
+    <t>7354b235-763d-4031-a92b-17249e674c94</t>
+  </si>
+  <si>
     <t>Fintech Leaders</t>
   </si>
   <si>
     <t>contact6@fintechleaders.com</t>
   </si>
   <si>
+    <t>002023/01/20</t>
+  </si>
+  <si>
+    <t>5027f96e-1544-4992-848e-b8a3f56ccf4e</t>
+  </si>
+  <si>
     <t>HealthTech Group</t>
   </si>
   <si>
     <t>contact7@healthtech.com</t>
   </si>
   <si>
+    <t>002023/01/21</t>
+  </si>
+  <si>
+    <t>d1c5e2d9-394b-43a6-8c56-d8f19a59b25e</t>
+  </si>
+  <si>
     <t>EduTech Innovators</t>
   </si>
   <si>
     <t>contact8@edutech.com</t>
   </si>
   <si>
+    <t>002023/01/22</t>
+  </si>
+  <si>
+    <t>6b07b6a3-60e6-453d-b93c-726d17445f29</t>
+  </si>
+  <si>
     <t>Smart Homes Inc.</t>
   </si>
   <si>
     <t>contact9@smarthomes.com</t>
   </si>
   <si>
+    <t>002023/01/23</t>
+  </si>
+  <si>
+    <t>1e16a30c-bdbc-44b6-882d-e1d58e5f7f3b</t>
+  </si>
+  <si>
     <t>AutoTech Solutions</t>
   </si>
   <si>
     <t>contact10@autotech.com</t>
   </si>
   <si>
+    <t>002023/01/24</t>
+  </si>
+  <si>
+    <t>aae3c38e-2da5-4ba8-bc2b-b843f4ed6e50</t>
+  </si>
+  <si>
     <t>Space Explorers</t>
   </si>
   <si>
     <t>contact11@spaceexplorers.com</t>
   </si>
   <si>
+    <t>002023/01/25</t>
+  </si>
+  <si>
+    <t>e5ad76be-bcdc-43a2-a8c5-73c1a2eec27e</t>
+  </si>
+  <si>
     <t>BioTech Innovations</t>
   </si>
   <si>
     <t>contact12@biotech.com</t>
   </si>
   <si>
+    <t>002023/01/26</t>
+  </si>
+  <si>
+    <t>57a6586a-7ef2-4d67-839b-4a8a15970848</t>
+  </si>
+  <si>
     <t>Quantum Computing</t>
   </si>
   <si>
     <t>contact13@quantumcomputing.com</t>
   </si>
   <si>
+    <t>002023/01/27</t>
+  </si>
+  <si>
+    <t>a95839d2-780b-4484-9955-52c2c16fa46f</t>
+  </si>
+  <si>
     <t>Cybersecurity Pros</t>
   </si>
   <si>
     <t>contact14@cyberpros.com</t>
   </si>
   <si>
+    <t>002023/01/28</t>
+  </si>
+  <si>
+    <t>8ffb5d76-4954-4e18-8f5f-8243827fa212</t>
+  </si>
+  <si>
     <t>Robotics Ventures</t>
   </si>
   <si>
     <t>contact15@roboticsventures.com</t>
   </si>
   <si>
+    <t>002023/01/29</t>
+  </si>
+  <si>
+    <t>1f5d9c9b-49f0-4f23-85c1-74c1b8b4e21f</t>
+  </si>
+  <si>
     <t>Blockchain Pioneers</t>
   </si>
   <si>
     <t>contact16@blockchain.com</t>
   </si>
   <si>
+    <t>002023/01/30</t>
+  </si>
+  <si>
+    <t>66e56de0-623a-4b40-a498-0b3a77f04c16</t>
+  </si>
+  <si>
     <t>AgriTech Innovators</t>
   </si>
   <si>
     <t>contact17@agritech.com</t>
   </si>
   <si>
+    <t>002023/01/31</t>
+  </si>
+  <si>
+    <t>493c2566-5533-476d-8a13-c4312a0a2f8b</t>
+  </si>
+  <si>
     <t>Digital Nomads</t>
   </si>
   <si>
     <t>contact18@digitalnomads.com</t>
   </si>
   <si>
+    <t>002023/02/01</t>
+  </si>
+  <si>
+    <t>728ea0fb-c5e5-4f23-a7ff-1b6f88b1d5f6</t>
+  </si>
+  <si>
     <t>AI Healthcare</t>
   </si>
   <si>
     <t>contact19@aihealthcare.com</t>
   </si>
   <si>
+    <t>002023/02/02</t>
+  </si>
+  <si>
+    <t>4f03b878-8be8-4f6b-a5e6-129d42bf0b34</t>
+  </si>
+  <si>
     <t>E-Commerce Wizards</t>
   </si>
   <si>
     <t>contact20@ecommerce.com</t>
   </si>
   <si>
+    <t>002023/02/03</t>
+  </si>
+  <si>
+    <t>8be2454b-7a74-4dbe-bd53-b650e1a5a2b4</t>
+  </si>
+  <si>
     <t>VR/AR Experiences</t>
   </si>
   <si>
     <t>contact21@vrexperiences.com</t>
   </si>
   <si>
+    <t>002023/02/04</t>
+  </si>
+  <si>
+    <t>acd4b8fb-f9cb-4139-990e-1e962b7a88fa</t>
+  </si>
+  <si>
     <t>Autonomous Vehicles</t>
   </si>
   <si>
     <t>contact22@autovehicles.com</t>
   </si>
   <si>
+    <t>002023/02/05</t>
+  </si>
+  <si>
+    <t>92e28dfc-9f74-41a4-9d91-e77a3d5a1c3b</t>
+  </si>
+  <si>
     <t>Fintech Ventures</t>
   </si>
   <si>
     <t>contact23@fintechventures.com</t>
   </si>
   <si>
+    <t>002023/02/06</t>
+  </si>
+  <si>
+    <t>5e79a6f3-5c49-4c47-9578-2e1a2b53c9fc</t>
+  </si>
+  <si>
     <t>Renewable Energy</t>
   </si>
   <si>
     <t>contact24@renewable.com</t>
   </si>
   <si>
+    <t>002023/02/07</t>
+  </si>
+  <si>
+    <t>c41d7c1f-f70c-4d42-94f3-2a4f3d4e2f94</t>
+  </si>
+  <si>
     <t>SpaceTech Partners</t>
   </si>
   <si>
     <t>contact25@spacetech.com</t>
   </si>
   <si>
+    <t>002023/02/08</t>
+  </si>
+  <si>
+    <t>9f61743a-2a4f-4bc5-89e9-5c0b75607b6a</t>
+  </si>
+  <si>
     <t>Smart City Projects</t>
   </si>
   <si>
     <t>contact26@smartcity.com</t>
   </si>
   <si>
+    <t>002023/02/09</t>
+  </si>
+  <si>
+    <t>aab312df-2e45-4d6b-b357-cc54104ad2b9</t>
+  </si>
+  <si>
     <t>AI Research Labs</t>
   </si>
   <si>
     <t>contact27@airesearch.com</t>
   </si>
   <si>
+    <t>002023/02/10</t>
+  </si>
+  <si>
+    <t>4e25474e-1a12-409f-9207-531c28470c6a</t>
+  </si>
+  <si>
     <t>Crypto Innovators</t>
   </si>
   <si>
     <t>contact28@crypto.com</t>
   </si>
   <si>
+    <t>002023/02/11</t>
+  </si>
+  <si>
+    <t>3df36be5-493d-4915-8fc3-4ed23d742d86</t>
+  </si>
+  <si>
     <t>GreenTech Solutions</t>
   </si>
   <si>
     <t>contact29@greentech.com</t>
   </si>
   <si>
+    <t>002023/02/12</t>
+  </si>
+  <si>
+    <t>a75b6f3e-542b-40f2-a129-4a9c72a86e7e</t>
+  </si>
+  <si>
     <t>Digital Transformation</t>
   </si>
   <si>
     <t>contact30@digitaltrans.com</t>
   </si>
   <si>
+    <t>002023/02/13</t>
+  </si>
+  <si>
+    <t>f3b7e5a2-38a9-4a9f-8e79-fb2a2a7c7f93</t>
+  </si>
+  <si>
     <t>AI Financials</t>
   </si>
   <si>
     <t>contact31@aifinancials.com</t>
   </si>
   <si>
+    <t>002023/02/14</t>
+  </si>
+  <si>
+    <t>bcb3759d-c9a7-4fa6-9a74-72a4c5b3c6ae</t>
+  </si>
+  <si>
     <t>Quantum Ventures</t>
   </si>
   <si>
     <t>contact32@quantumventures.com</t>
   </si>
   <si>
+    <t>002023/02/15</t>
+  </si>
+  <si>
+    <t>4e02d7af-2b47-48d5-9d7f-3b85f3a3c6f3</t>
+  </si>
+  <si>
     <t>VR Innovators</t>
   </si>
   <si>
     <t>contact33@vrinnovators.com</t>
   </si>
   <si>
+    <t>002023/02/16</t>
+  </si>
+  <si>
+    <t>85a3c6d5-c94a-49d6-b8f4-0f39b3c7c9fe</t>
+  </si>
+  <si>
     <t>AutoTech Innovators</t>
   </si>
   <si>
     <t>contact34@autotechinnovators.com</t>
   </si>
   <si>
+    <t>002023/02/17</t>
+  </si>
+  <si>
+    <t>71f5b2e7-3c14-41d5-b8f5-4b9f4a7c2c7f</t>
+  </si>
+  <si>
     <t>AI Solutions</t>
   </si>
   <si>
     <t>contact35@aisolutions.com</t>
   </si>
   <si>
+    <t>002023/02/18</t>
+  </si>
+  <si>
+    <t>4b78c3e9-5a4e-43f7-bc47-1a2b5a6c2d7f</t>
+  </si>
+  <si>
     <t>Fintech Masters</t>
   </si>
   <si>
     <t>contact36@fintechmasters.com</t>
   </si>
   <si>
+    <t>002023/02/19</t>
+  </si>
+  <si>
+    <t>67f2b6f7-3c15-45f9-8b76-3f9a5b7f3d9a</t>
+  </si>
+  <si>
     <t>Renewable Innovations</t>
   </si>
   <si>
     <t>contact37@renewableinnovations.com</t>
   </si>
   <si>
+    <t>002023/02/20</t>
+  </si>
+  <si>
+    <t>89b6f3e7-4c27-49f3-b7a2-2f39a5c7c8f3</t>
+  </si>
+  <si>
     <t>Cybersecurity Labs</t>
   </si>
   <si>
     <t>contact38@cyberlabs.com</t>
   </si>
   <si>
+    <t>002023/02/21</t>
+  </si>
+  <si>
+    <t>6c8f2d3b-5d4a-4a8b-946c-2e9a4b5c8f47</t>
+  </si>
+  <si>
     <t>HealthTech Ventures</t>
   </si>
   <si>
     <t>contact39@healthventures.com</t>
   </si>
   <si>
+    <t>002023/02/22</t>
+  </si>
+  <si>
+    <t>74f3c2d8-4a3d-40f8-b5c7-2a6b4f3d7f89</t>
+  </si>
+  <si>
     <t>AI Energy Solutions</t>
   </si>
   <si>
     <t>contact40@aienergy.com</t>
   </si>
   <si>
+    <t>002023/02/23</t>
+  </si>
+  <si>
+    <t>5d7f2e4a-6b3c-4b6f-9f47-1c8b5e3c7f9a</t>
+  </si>
+  <si>
     <t>VR Labs</t>
   </si>
   <si>
     <t>contact41@vrlabs.com</t>
   </si>
   <si>
+    <t>002023/02/24</t>
+  </si>
+  <si>
+    <t>82f9c3e4-5d7f-44b8-b5c7-2a9f4d7c8b6f</t>
+  </si>
+  <si>
     <t>AI Enterprises</t>
   </si>
   <si>
     <t>contact42@aienterprises.com</t>
   </si>
   <si>
+    <t>002023/02/25</t>
+  </si>
+  <si>
+    <t>7f5c4d8e-6b3c-4f6b-8f4a-3b9f4e5c7d8f</t>
+  </si>
+  <si>
     <t>Blockchain Masters</t>
   </si>
   <si>
     <t>contact43@blockchainmasters.com</t>
   </si>
   <si>
+    <t>002023/02/26</t>
+  </si>
+  <si>
+    <t>9a8f6c5d-3e2a-4f9b-8f4c-1a7d4c5b7e8f</t>
+  </si>
+  <si>
     <t>GreenTech Ventures</t>
   </si>
   <si>
     <t>contact44@greentechventures.com</t>
   </si>
   <si>
+    <t>002023/02/27</t>
+  </si>
+  <si>
+    <t>7b3e4f8d-9a6b-4d7f-b4f9-2a8f4c5d7e9b</t>
+  </si>
+  <si>
     <t>EduTech Leaders</t>
   </si>
   <si>
     <t>contact45@edutechleaders.com</t>
   </si>
   <si>
+    <t>002023/02/28</t>
+  </si>
+  <si>
+    <t>8d6f7e5c-3c2a-4b9f-8f5a-3d7f4c5b6a9e</t>
+  </si>
+  <si>
     <t>AI in Finance</t>
   </si>
   <si>
     <t>contact46@aiinfinance.com</t>
   </si>
   <si>
+    <t>002023/03/01</t>
+  </si>
+  <si>
+    <t>6a5b3c8f-7d2e-4b9f-8f5d-2f9b4d5c7e8f</t>
+  </si>
+  <si>
     <t>Smart Tech</t>
   </si>
   <si>
     <t>contact47@smarttech.com</t>
   </si>
   <si>
+    <t>002023/03/02</t>
+  </si>
+  <si>
+    <t>7c8f4d6e-3a2f-4f8b-9f5c-1d7e4c5b8f9a</t>
+  </si>
+  <si>
     <t>E-Commerce Innovators</t>
   </si>
   <si>
     <t>contact48@ecommerceinnovators.com</t>
   </si>
   <si>
+    <t>002023/03/03</t>
+  </si>
+  <si>
+    <t>8e9f5d3c-2b4a-4f6b-8f9c-3a7e4c5d7b8f</t>
+  </si>
+  <si>
     <t>Space Ventures</t>
   </si>
   <si>
     <t>contact49@spaceventures.com</t>
   </si>
   <si>
+    <t>002023/03/04</t>
+  </si>
+  <si>
+    <t>9b7f4d8c-3e2f-4f9b-8f5a-2c7e4b5d6a9f</t>
+  </si>
+  <si>
     <t>Robotics Innovators</t>
   </si>
   <si>
     <t>contact50@roboticsinnovators.com</t>
   </si>
   <si>
-    <t>Test Passed</t>
-  </si>
-  <si>
-    <t>68c53a7b-2b9e-4dbe-a536-4d1a2f27a0b7</t>
-  </si>
-  <si>
-    <t>77af89a2-7c76-4263-a8ee-2b25541f89af</t>
-  </si>
-  <si>
-    <t>f5a92c1a-59b0-496f-8d17-64bdf59d3f6a</t>
-  </si>
-  <si>
-    <t>c1c1fbb6-9a94-41b7-94f8-7a621aa1a7b6</t>
-  </si>
-  <si>
-    <t>9e58f2fa-d8a8-46c7-988a-2bb0c9c78f94</t>
-  </si>
-  <si>
-    <t>7354b235-763d-4031-a92b-17249e674c94</t>
-  </si>
-  <si>
-    <t>5027f96e-1544-4992-848e-b8a3f56ccf4e</t>
-  </si>
-  <si>
-    <t>d1c5e2d9-394b-43a6-8c56-d8f19a59b25e</t>
-  </si>
-  <si>
-    <t>6b07b6a3-60e6-453d-b93c-726d17445f29</t>
-  </si>
-  <si>
-    <t>1e16a30c-bdbc-44b6-882d-e1d58e5f7f3b</t>
-  </si>
-  <si>
-    <t>aae3c38e-2da5-4ba8-bc2b-b843f4ed6e50</t>
-  </si>
-  <si>
-    <t>e5ad76be-bcdc-43a2-a8c5-73c1a2eec27e</t>
-  </si>
-  <si>
-    <t>57a6586a-7ef2-4d67-839b-4a8a15970848</t>
-  </si>
-  <si>
-    <t>a95839d2-780b-4484-9955-52c2c16fa46f</t>
-  </si>
-  <si>
-    <t>8ffb5d76-4954-4e18-8f5f-8243827fa212</t>
-  </si>
-  <si>
-    <t>1f5d9c9b-49f0-4f23-85c1-74c1b8b4e21f</t>
-  </si>
-  <si>
-    <t>66e56de0-623a-4b40-a498-0b3a77f04c16</t>
-  </si>
-  <si>
-    <t>493c2566-5533-476d-8a13-c4312a0a2f8b</t>
-  </si>
-  <si>
-    <t>728ea0fb-c5e5-4f23-a7ff-1b6f88b1d5f6</t>
-  </si>
-  <si>
-    <t>4f03b878-8be8-4f6b-a5e6-129d42bf0b34</t>
-  </si>
-  <si>
-    <t>8be2454b-7a74-4dbe-bd53-b650e1a5a2b4</t>
-  </si>
-  <si>
-    <t>acd4b8fb-f9cb-4139-990e-1e962b7a88fa</t>
-  </si>
-  <si>
-    <t>92e28dfc-9f74-41a4-9d91-e77a3d5a1c3b</t>
-  </si>
-  <si>
-    <t>5e79a6f3-5c49-4c47-9578-2e1a2b53c9fc</t>
-  </si>
-  <si>
-    <t>c41d7c1f-f70c-4d42-94f3-2a4f3d4e2f94</t>
-  </si>
-  <si>
-    <t>9f61743a-2a4f-4bc5-89e9-5c0b75607b6a</t>
-  </si>
-  <si>
-    <t>aab312df-2e45-4d6b-b357-cc54104ad2b9</t>
-  </si>
-  <si>
-    <t>4e25474e-1a12-409f-9207-531c28470c6a</t>
-  </si>
-  <si>
-    <t>3df36be5-493d-4915-8fc3-4ed23d742d86</t>
-  </si>
-  <si>
-    <t>a75b6f3e-542b-40f2-a129-4a9c72a86e7e</t>
-  </si>
-  <si>
-    <t>f3b7e5a2-38a9-4a9f-8e79-fb2a2a7c7f93</t>
-  </si>
-  <si>
-    <t>bcb3759d-c9a7-4fa6-9a74-72a4c5b3c6ae</t>
-  </si>
-  <si>
-    <t>4e02d7af-2b47-48d5-9d7f-3b85f3a3c6f3</t>
-  </si>
-  <si>
-    <t>85a3c6d5-c94a-49d6-b8f4-0f39b3c7c9fe</t>
-  </si>
-  <si>
-    <t>71f5b2e7-3c14-41d5-b8f5-4b9f4a7c2c7f</t>
-  </si>
-  <si>
-    <t>4b78c3e9-5a4e-43f7-bc47-1a2b5a6c2d7f</t>
-  </si>
-  <si>
-    <t>67f2b6f7-3c15-45f9-8b76-3f9a5b7f3d9a</t>
-  </si>
-  <si>
-    <t>89b6f3e7-4c27-49f3-b7a2-2f39a5c7c8f3</t>
-  </si>
-  <si>
-    <t>6c8f2d3b-5d4a-4a8b-946c-2e9a4b5c8f47</t>
-  </si>
-  <si>
-    <t>74f3c2d8-4a3d-40f8-b5c7-2a6b4f3d7f89</t>
-  </si>
-  <si>
-    <t>5d7f2e4a-6b3c-4b6f-9f47-1c8b5e3c7f9a</t>
-  </si>
-  <si>
-    <t>82f9c3e4-5d7f-44b8-b5c7-2a9f4d7c8b6f</t>
-  </si>
-  <si>
-    <t>7f5c4d8e-6b3c-4f6b-8f4a-3b9f4e5c7d8f</t>
-  </si>
-  <si>
-    <t>9a8f6c5d-3e2a-4f9b-8f4c-1a7d4c5b7e8f</t>
-  </si>
-  <si>
-    <t>7b3e4f8d-9a6b-4d7f-b4f9-2a8f4c5d7e9b</t>
-  </si>
-  <si>
-    <t>8d6f7e5c-3c2a-4b9f-8f5a-3d7f4c5b6a9e</t>
-  </si>
-  <si>
-    <t>6a5b3c8f-7d2e-4b9f-8f5d-2f9b4d5c7e8f</t>
-  </si>
-  <si>
-    <t>7c8f4d6e-3a2f-4f8b-9f5c-1d7e4c5b8f9a</t>
-  </si>
-  <si>
-    <t>8e9f5d3c-2b4a-4f6b-8f9c-3a7e4c5d7b8f</t>
-  </si>
-  <si>
-    <t>9b7f4d8c-3e2f-4f9b-8f5a-2c7e4b5d6a9f</t>
+    <t>002023/03/05</t>
   </si>
   <si>
     <t>ProjectID</t>
@@ -937,7 +1087,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -974,7 +1124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -987,6 +1137,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1324,18 +1477,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3CC1F3F-070D-4831-8C1F-2CBF832928B6}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47:D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="3" max="3" width="39.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1349,707 +1502,708 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="29.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="29.25">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="29.25">
+      <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="29.25">
+      <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="29.25">
+      <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="29.25">
+      <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="29.25">
+      <c r="A14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="29.25">
+      <c r="A18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="29.25">
+      <c r="A19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="29.25">
+      <c r="A22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2">
-        <v>44941</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2">
-        <v>44942</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2">
-        <v>44943</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="D27" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2">
-        <v>44944</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    </row>
+    <row r="28" spans="1:4" ht="29.25">
+      <c r="A28" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="2">
-        <v>44945</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2">
-        <v>44946</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="2">
-        <v>44947</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="D28" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="2">
-        <v>44948</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    </row>
+    <row r="29" spans="1:4" ht="29.25">
+      <c r="A29" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="2">
-        <v>44949</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="2">
-        <v>44950</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="2">
-        <v>44951</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="D29" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="2">
-        <v>44952</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="2">
-        <v>44953</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="2">
-        <v>44954</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="2">
-        <v>44955</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="D30" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="2">
-        <v>44956</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="2">
-        <v>44957</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="2">
-        <v>44958</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="2">
-        <v>44959</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="D31" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="2">
-        <v>44960</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="2">
-        <v>44961</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="2">
-        <v>44962</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="2">
-        <v>44963</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="D32" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" s="2">
-        <v>44964</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" s="2">
-        <v>44965</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="2">
-        <v>44966</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="2">
-        <v>44967</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="D33" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="2">
-        <v>44968</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="2">
-        <v>44969</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="2">
-        <v>44970</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D32" s="2">
-        <v>44971</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="D34" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" s="2">
-        <v>44972</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34" s="2">
-        <v>44973</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="C35" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="2">
-        <v>44974</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>72</v>
+        <v>142</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D36" s="2">
-        <v>44975</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>74</v>
+        <v>146</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D37" s="2">
-        <v>44976</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>76</v>
+        <v>150</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D38" s="2">
-        <v>44977</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>78</v>
+        <v>154</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D39" s="2">
-        <v>44978</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>80</v>
+        <v>158</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D40" s="2">
-        <v>44979</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>82</v>
+        <v>162</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D41" s="2">
-        <v>44980</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>84</v>
+        <v>166</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D42" s="2">
-        <v>44981</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>86</v>
+        <v>170</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D43" s="2">
-        <v>44982</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>147</v>
+        <v>173</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>88</v>
+        <v>174</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D44" s="2">
-        <v>44983</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
-        <v>148</v>
+        <v>177</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>90</v>
+        <v>178</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D45" s="2">
-        <v>44984</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
-        <v>149</v>
+        <v>181</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D46" s="2">
-        <v>44985</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="1" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>94</v>
+        <v>186</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D47" s="2">
-        <v>44986</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>96</v>
+        <v>190</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D48" s="2">
-        <v>44987</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
-        <v>152</v>
+        <v>193</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>98</v>
+        <v>194</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D49" s="2">
-        <v>44988</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>153</v>
+        <v>197</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>100</v>
+        <v>198</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D50" s="2">
-        <v>44989</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>154</v>
+        <v>201</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>102</v>
+        <v>202</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D51" s="2">
-        <v>44990</v>
+        <v>203</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -2061,11 +2215,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D331589-AA9D-4074-9BAA-5A515B94893D}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="40.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="40.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
@@ -2074,927 +2228,927 @@
     <col min="6" max="6" width="38.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>155</v>
+        <v>205</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>157</v>
+        <v>207</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>158</v>
+        <v>208</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>159</v>
+        <v>209</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>160</v>
+        <v>210</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>161</v>
+        <v>211</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>162</v>
+        <v>212</v>
       </c>
       <c r="D2" s="2">
         <v>44958</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>164</v>
+        <v>214</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>165</v>
+        <v>215</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>166</v>
+        <v>216</v>
       </c>
       <c r="D3" s="2">
         <v>44959</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>167</v>
+        <v>217</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>168</v>
+        <v>218</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>169</v>
+        <v>219</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>170</v>
+        <v>220</v>
       </c>
       <c r="D4" s="2">
         <v>44960</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>171</v>
+        <v>221</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>172</v>
+        <v>222</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>173</v>
+        <v>223</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>174</v>
+        <v>224</v>
       </c>
       <c r="D5" s="2">
         <v>44961</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>175</v>
+        <v>225</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>177</v>
+        <v>227</v>
       </c>
       <c r="D6" s="2">
         <v>44962</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>178</v>
+        <v>228</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>179</v>
+        <v>229</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>180</v>
+        <v>230</v>
       </c>
       <c r="D7" s="2">
         <v>44963</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>167</v>
+        <v>217</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>181</v>
+        <v>231</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>182</v>
+        <v>232</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>183</v>
+        <v>233</v>
       </c>
       <c r="D8" s="2">
         <v>44964</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30">
       <c r="A9" s="1" t="s">
-        <v>184</v>
+        <v>234</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>185</v>
+        <v>235</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>186</v>
+        <v>236</v>
       </c>
       <c r="D9" s="2">
         <v>44965</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>187</v>
+        <v>237</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>188</v>
+        <v>238</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>189</v>
+        <v>239</v>
       </c>
       <c r="D10" s="2">
         <v>44966</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>171</v>
+        <v>221</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>190</v>
+        <v>240</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>191</v>
+        <v>241</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>192</v>
+        <v>242</v>
       </c>
       <c r="D11" s="2">
         <v>44967</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>193</v>
+        <v>243</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>194</v>
+        <v>244</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>195</v>
+        <v>245</v>
       </c>
       <c r="D12" s="2">
         <v>44968</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>196</v>
+        <v>246</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>197</v>
+        <v>247</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>198</v>
+        <v>248</v>
       </c>
       <c r="D13" s="2">
         <v>44969</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>199</v>
+        <v>249</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>201</v>
+        <v>251</v>
       </c>
       <c r="D14" s="2">
         <v>44970</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="1" t="s">
-        <v>202</v>
+        <v>252</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>203</v>
+        <v>253</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>204</v>
+        <v>254</v>
       </c>
       <c r="D15" s="2">
         <v>44971</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="1" t="s">
-        <v>205</v>
+        <v>255</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>206</v>
+        <v>256</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>207</v>
+        <v>257</v>
       </c>
       <c r="D16" s="2">
         <v>44972</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>167</v>
+        <v>217</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>208</v>
+        <v>258</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>209</v>
+        <v>259</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>210</v>
+        <v>260</v>
       </c>
       <c r="D17" s="2">
         <v>44973</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>171</v>
+        <v>221</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>211</v>
+        <v>261</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>212</v>
+        <v>262</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>213</v>
+        <v>263</v>
       </c>
       <c r="D18" s="2">
         <v>44974</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>214</v>
+        <v>264</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>215</v>
+        <v>265</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>216</v>
+        <v>266</v>
       </c>
       <c r="D19" s="2">
         <v>44975</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>167</v>
+        <v>217</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>217</v>
+        <v>267</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>218</v>
+        <v>268</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>219</v>
+        <v>269</v>
       </c>
       <c r="D20" s="2">
         <v>44976</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>220</v>
+        <v>270</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>221</v>
+        <v>271</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>222</v>
+        <v>272</v>
       </c>
       <c r="D21" s="2">
         <v>44977</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>223</v>
+        <v>273</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>224</v>
+        <v>274</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>225</v>
+        <v>275</v>
       </c>
       <c r="D22" s="2">
         <v>44978</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30">
       <c r="A23" s="1" t="s">
-        <v>226</v>
+        <v>276</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>227</v>
+        <v>277</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>228</v>
+        <v>278</v>
       </c>
       <c r="D23" s="2">
         <v>44979</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>229</v>
+        <v>279</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>230</v>
+        <v>280</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>231</v>
+        <v>281</v>
       </c>
       <c r="D24" s="2">
         <v>44980</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>232</v>
+        <v>282</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>233</v>
+        <v>283</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>234</v>
+        <v>284</v>
       </c>
       <c r="D25" s="2">
         <v>44981</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>171</v>
+        <v>221</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>235</v>
+        <v>285</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>236</v>
+        <v>286</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>237</v>
+        <v>287</v>
       </c>
       <c r="D26" s="2">
         <v>44982</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>238</v>
+        <v>288</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>239</v>
+        <v>289</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>240</v>
+        <v>290</v>
       </c>
       <c r="D27" s="2">
         <v>44983</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30">
       <c r="A28" s="1" t="s">
-        <v>241</v>
+        <v>291</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>242</v>
+        <v>292</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>243</v>
+        <v>293</v>
       </c>
       <c r="D28" s="2">
         <v>44984</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>244</v>
+        <v>294</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>245</v>
+        <v>295</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>246</v>
+        <v>296</v>
       </c>
       <c r="D29" s="2">
         <v>44985</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>247</v>
+        <v>297</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>248</v>
+        <v>298</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>249</v>
+        <v>299</v>
       </c>
       <c r="D30" s="2">
         <v>44986</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>251</v>
+        <v>301</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>252</v>
+        <v>302</v>
       </c>
       <c r="D31" s="2">
         <v>44987</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>167</v>
+        <v>217</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>253</v>
+        <v>303</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>254</v>
+        <v>304</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>255</v>
+        <v>305</v>
       </c>
       <c r="D32" s="2">
         <v>44988</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>171</v>
+        <v>221</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="30">
       <c r="A33" s="1" t="s">
-        <v>256</v>
+        <v>306</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>257</v>
+        <v>307</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>258</v>
+        <v>308</v>
       </c>
       <c r="D33" s="2">
         <v>44989</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>259</v>
+        <v>309</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>260</v>
+        <v>310</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>261</v>
+        <v>311</v>
       </c>
       <c r="D34" s="2">
         <v>44990</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
-        <v>262</v>
+        <v>312</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>263</v>
+        <v>313</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>264</v>
+        <v>314</v>
       </c>
       <c r="D35" s="2">
         <v>44991</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
-        <v>265</v>
+        <v>315</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>266</v>
+        <v>316</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>267</v>
+        <v>317</v>
       </c>
       <c r="D36" s="2">
         <v>44992</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
-        <v>268</v>
+        <v>318</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>269</v>
+        <v>319</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>270</v>
+        <v>320</v>
       </c>
       <c r="D37" s="2">
         <v>44993</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
-        <v>271</v>
+        <v>321</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>272</v>
+        <v>322</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="D38" s="2">
         <v>44994</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="30">
       <c r="A39" s="1" t="s">
-        <v>274</v>
+        <v>324</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>275</v>
+        <v>325</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>276</v>
+        <v>326</v>
       </c>
       <c r="D39" s="2">
         <v>44995</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>167</v>
+        <v>217</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="30">
       <c r="A40" s="1" t="s">
-        <v>277</v>
+        <v>327</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>278</v>
+        <v>328</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>279</v>
+        <v>329</v>
       </c>
       <c r="D40" s="2">
         <v>44996</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>171</v>
+        <v>221</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
-        <v>280</v>
+        <v>330</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>281</v>
+        <v>331</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>282</v>
+        <v>332</v>
       </c>
       <c r="D41" s="2">
         <v>44997</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="1" t="s">
-        <v>283</v>
+        <v>333</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>284</v>
+        <v>334</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>285</v>
+        <v>335</v>
       </c>
       <c r="D42" s="2">
         <v>44998</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="30">
       <c r="A43" s="1" t="s">
-        <v>286</v>
+        <v>336</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>287</v>
+        <v>337</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>288</v>
+        <v>338</v>
       </c>
       <c r="D43" s="2">
         <v>44999</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="1" t="s">
-        <v>289</v>
+        <v>339</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>290</v>
+        <v>340</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>291</v>
+        <v>341</v>
       </c>
       <c r="D44" s="2">
         <v>45000</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="1" t="s">
-        <v>292</v>
+        <v>342</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>293</v>
+        <v>343</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>294</v>
+        <v>344</v>
       </c>
       <c r="D45" s="2">
         <v>45001</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="1" t="s">
-        <v>295</v>
+        <v>345</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>296</v>
+        <v>346</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>297</v>
+        <v>347</v>
       </c>
       <c r="D46" s="2">
         <v>45002</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>117</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>